<commit_message>
add gen UIPage cs
</commit_message>
<xml_diff>
--- a/Excel2Unity/Excel/UI.xlsx
+++ b/Excel2Unity/Excel/UI.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ADBBD8-676E-4DB1-A74F-CB70FD9EDB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE56852B-B6E9-46A4-9298-17DEC946C7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>CS</t>
   </si>
@@ -125,6 +125,22 @@
   </si>
   <si>
     <t>enum:UIMaskType(None,OnlyMask,MaskClickClose,TransparentMask,TransparentClickMask)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UIPage名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameOver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameStart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uiPage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -622,26 +638,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.125" customWidth="1"/>
-    <col min="3" max="3" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="25.625" customWidth="1"/>
-    <col min="8" max="9" width="24.375" customWidth="1"/>
-    <col min="10" max="10" width="38.5" customWidth="1"/>
-    <col min="11" max="12" width="41.375" customWidth="1"/>
+    <col min="1" max="3" width="21.08984375" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="89.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.6328125" customWidth="1"/>
+    <col min="9" max="10" width="24.36328125" customWidth="1"/>
+    <col min="11" max="11" width="38.453125" customWidth="1"/>
+    <col min="12" max="13" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -649,30 +665,33 @@
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -680,16 +699,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="6" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -697,21 +719,24 @@
         <v>9</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -719,16 +744,19 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -736,16 +764,19 @@
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -756,9 +787,12 @@
         <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -779,7 +813,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:XFD2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"C,S,CS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:XFD3" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:XFD3" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"int,float,bool,string,list[int],list[float],list[string],map[int|int],map[int|float],map[int|string],map[string|int],map[string|float],map[string|string]"</formula1>
     </dataValidation>
   </dataValidations>
@@ -794,7 +828,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -807,7 +841,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fixed and remove uiInfo in uiPath
</commit_message>
<xml_diff>
--- a/Excel2Unity/Excel/UI.xlsx
+++ b/Excel2Unity/Excel/UI.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE56852B-B6E9-46A4-9298-17DEC946C7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58260203-3475-420E-9474-532511CBD80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>CS</t>
   </si>
@@ -96,14 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>预留界面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>desseedli+osirisgu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ComFull</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,6 +133,34 @@
   </si>
   <si>
     <t>uiPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遮罩界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaskUI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Canvas/MaskUI.prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MessageUI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Canvas/MessageUI.prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaskClickClose</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -267,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,6 +314,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -638,11 +661,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -665,7 +688,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>11</v>
@@ -705,10 +728,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -719,16 +742,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -744,16 +767,16 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -764,16 +787,16 @@
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -781,19 +804,39 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>